<commit_message>
Reports handed in commit
</commit_message>
<xml_diff>
--- a/Rapport resourcer/Tidsplan - Realiseret.xlsx
+++ b/Rapport resourcer/Tidsplan - Realiseret.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mg\Desktop\Svendeproeve\Rapport resourcer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9BC5A3-B341-4A97-992A-520AA4748A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A049F47-1A56-4322-BE80-948D90104CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -217,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="67">
+  <fills count="70">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -752,6 +752,24 @@
       <patternFill patternType="darkUp">
         <fgColor theme="5" tint="0.39994506668294322"/>
         <bgColor theme="0" tint="-0.34998626667073579"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkUp">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkUp">
+        <fgColor theme="7" tint="0.39994506668294322"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkUp">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -1061,7 +1079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1161,8 +1179,11 @@
     <xf numFmtId="0" fontId="0" fillId="64" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="65" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="66" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="55" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="56" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="67" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="68" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="69" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1452,7 +1473,7 @@
   <dimension ref="B1:AG29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE29" sqref="AE29"/>
+      <selection activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,12 +1645,12 @@
       <c r="Y4" s="79"/>
       <c r="Z4" s="79"/>
       <c r="AA4" s="79"/>
-      <c r="AB4" s="89"/>
+      <c r="AB4" s="90"/>
       <c r="AC4" s="69"/>
       <c r="AD4" s="72"/>
       <c r="AE4" s="86"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="2"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="93"/>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B5" s="64"/>
@@ -1808,7 +1829,7 @@
       <c r="AC9" s="69"/>
       <c r="AD9" s="72"/>
       <c r="AE9" s="72"/>
-      <c r="AF9" s="69"/>
+      <c r="AF9" s="90"/>
       <c r="AG9" s="2"/>
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.25">
@@ -1843,8 +1864,8 @@
       <c r="AB10" s="69"/>
       <c r="AC10" s="69"/>
       <c r="AD10" s="72"/>
-      <c r="AE10" s="72"/>
-      <c r="AF10" s="69"/>
+      <c r="AE10" s="86"/>
+      <c r="AF10" s="90"/>
       <c r="AG10" s="2"/>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
@@ -1880,7 +1901,7 @@
       <c r="AC11" s="69"/>
       <c r="AD11" s="72"/>
       <c r="AE11" s="72"/>
-      <c r="AF11" s="69"/>
+      <c r="AF11" s="90"/>
       <c r="AG11" s="2"/>
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.25">
@@ -1948,12 +1969,12 @@
       <c r="Y13" s="75"/>
       <c r="Z13" s="75"/>
       <c r="AA13" s="75"/>
-      <c r="AB13" s="90"/>
+      <c r="AB13" s="91"/>
       <c r="AC13" s="69"/>
       <c r="AD13" s="72"/>
       <c r="AE13" s="85"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="2"/>
+      <c r="AF13" s="91"/>
+      <c r="AG13" s="92"/>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B14" s="64"/>
@@ -2024,7 +2045,7 @@
       <c r="AC15" s="69"/>
       <c r="AD15" s="72"/>
       <c r="AE15" s="72"/>
-      <c r="AF15" s="69"/>
+      <c r="AF15" s="91"/>
       <c r="AG15" s="2"/>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.25">
@@ -2060,7 +2081,7 @@
       <c r="AC16" s="69"/>
       <c r="AD16" s="72"/>
       <c r="AE16" s="72"/>
-      <c r="AF16" s="69"/>
+      <c r="AF16" s="91"/>
       <c r="AG16" s="2"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.25">
@@ -2095,8 +2116,8 @@
       <c r="AB17" s="69"/>
       <c r="AC17" s="69"/>
       <c r="AD17" s="72"/>
-      <c r="AE17" s="72"/>
-      <c r="AF17" s="69"/>
+      <c r="AE17" s="85"/>
+      <c r="AF17" s="91"/>
       <c r="AG17" s="2"/>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.25">
@@ -2132,7 +2153,7 @@
       <c r="AC18" s="69"/>
       <c r="AD18" s="72"/>
       <c r="AE18" s="72"/>
-      <c r="AF18" s="69"/>
+      <c r="AF18" s="91"/>
       <c r="AG18" s="2"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.25">
@@ -2168,7 +2189,7 @@
       <c r="AC19" s="69"/>
       <c r="AD19" s="72"/>
       <c r="AE19" s="72"/>
-      <c r="AF19" s="69"/>
+      <c r="AF19" s="91"/>
       <c r="AG19" s="2"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.25">
@@ -2492,7 +2513,7 @@
       <c r="AC28" s="69"/>
       <c r="AD28" s="72"/>
       <c r="AE28" s="72"/>
-      <c r="AF28" s="69"/>
+      <c r="AF28" s="89"/>
       <c r="AG28" s="2"/>
     </row>
     <row r="29" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>